<commit_message>
Przerzuciłem nagrywanie głosu do osobnej klasy, dodałem parametr w klasie Excel, zwracany przez Morfeusza
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Dokumenty\Piter\III ROK\TechnologiaMowy\Projekt_II\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="23640" windowHeight="9795"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="23640" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="produkty" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>banan</t>
   </si>
@@ -30,12 +35,15 @@
   </si>
   <si>
     <t>chleb</t>
+  </si>
+  <si>
+    <t>truskawka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -74,6 +82,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -120,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,9 +168,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,6 +203,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -361,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -400,6 +418,11 @@
       </c>
       <c r="B5" s="1"/>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -407,11 +430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -441,6 +464,11 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
full working calorie count and file managing
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Dokumenty\Piter\III ROK\TechnologiaMowy\Projekt_II\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="23640" windowHeight="9795"/>
   </bookViews>
@@ -44,19 +39,19 @@
     <t>masło</t>
   </si>
   <si>
-    <t>ryż</t>
-  </si>
-  <si>
     <t>ilość</t>
   </si>
   <si>
     <t>waga</t>
+  </si>
+  <si>
+    <t>czekolada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -149,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,10 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,7 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -392,11 +385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -443,7 +436,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -453,7 +446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -508,7 +501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -519,42 +512,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>